<commit_message>
update query dues-in & dues-out
</commit_message>
<xml_diff>
--- a/kms/HIS-2396/HIS-2396 - Update Transaction Status List v0.2.xlsx
+++ b/kms/HIS-2396/HIS-2396 - Update Transaction Status List v0.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thanh.phamvan\Desktop\HIS-2396\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MySpace\PMS\kms\HIS-2396\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DE97CE-4DB5-4BBB-9F52-1EC9431D406A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B37856B-6C90-4CDA-88BD-2503E34B80BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{F92CBCCC-CE4E-451F-B585-C555BA546955}"/>
   </bookViews>
@@ -436,8 +436,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -448,20 +459,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,7 +786,7 @@
   <dimension ref="A1:AF72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,10 +819,10 @@
       <c r="E1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="18" t="s">
         <v>63</v>
       </c>
       <c r="H1" s="14">
@@ -909,7 +909,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="G2" s="28"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -927,7 +927,7 @@
       <c r="E3" s="13">
         <v>2</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -937,7 +937,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="G4" s="28"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -955,7 +955,7 @@
       <c r="E5" s="12">
         <v>2</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="22"/>
       <c r="K5">
         <v>0.25</v>
       </c>
@@ -964,7 +964,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -979,18 +979,18 @@
       <c r="E6" s="7">
         <v>0.25</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" s="23">
+      <c r="G6" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="26">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1003,13 +1003,13 @@
       <c r="E7" s="7">
         <v>0.25</v>
       </c>
-      <c r="G7" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L7" s="23"/>
+      <c r="G7" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1022,13 +1022,13 @@
       <c r="E8" s="7">
         <v>0.25</v>
       </c>
-      <c r="G8" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="23"/>
+      <c r="G8" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="7" t="s">
         <v>28</v>
       </c>
@@ -1041,13 +1041,13 @@
       <c r="E9" s="7">
         <v>0.25</v>
       </c>
-      <c r="G9" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L9" s="23"/>
+      <c r="G9" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
@@ -1060,13 +1060,13 @@
       <c r="E10" s="7">
         <v>0.25</v>
       </c>
-      <c r="G10" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L10" s="23"/>
+      <c r="G10" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
@@ -1079,13 +1079,13 @@
       <c r="E11" s="7">
         <v>0.25</v>
       </c>
-      <c r="G11" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="23"/>
+      <c r="G11" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1098,13 +1098,13 @@
       <c r="E12" s="7">
         <v>0.25</v>
       </c>
-      <c r="G12" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" s="23"/>
+      <c r="G12" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1117,10 +1117,10 @@
       <c r="E13" s="7">
         <v>0.25</v>
       </c>
-      <c r="G13" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L13" s="23"/>
+      <c r="G13" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="26"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1138,7 +1138,7 @@
       <c r="E14" s="11">
         <v>2</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="25" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1150,10 +1150,10 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="G15" s="25"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -1168,15 +1168,15 @@
       <c r="E16" s="16">
         <v>2</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="16" t="s">
         <v>37</v>
       </c>
@@ -1189,12 +1189,12 @@
       <c r="E17" s="16">
         <v>1</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="16" t="s">
         <v>38</v>
       </c>
@@ -1207,12 +1207,12 @@
       <c r="E18" s="16">
         <v>1</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="16" t="s">
         <v>17</v>
       </c>
@@ -1225,12 +1225,12 @@
       <c r="E19" s="16">
         <v>1</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1245,13 +1245,13 @@
       <c r="E20" s="16">
         <v>2</v>
       </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="25" t="s">
+      <c r="F20" s="24"/>
+      <c r="G20" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="16" t="s">
         <v>32</v>
       </c>
@@ -1264,12 +1264,12 @@
       <c r="E21" s="16">
         <v>1</v>
       </c>
-      <c r="G21" s="25" t="s">
+      <c r="G21" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="16" t="s">
         <v>23</v>
       </c>
@@ -1282,12 +1282,12 @@
       <c r="E22" s="16">
         <v>1</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -1302,10 +1302,10 @@
       <c r="E23" s="17">
         <v>2.25</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="19" t="s">
         <v>61</v>
       </c>
       <c r="H23">
@@ -1319,7 +1319,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="17" t="s">
         <v>30</v>
       </c>
@@ -1332,15 +1332,15 @@
       <c r="E24" s="17">
         <v>0.25</v>
       </c>
-      <c r="G24" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="J24" s="18">
+      <c r="G24" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="17" t="s">
         <v>23</v>
       </c>
@@ -1353,13 +1353,13 @@
       <c r="E25" s="17">
         <v>0.25</v>
       </c>
-      <c r="G25" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="J25" s="18"/>
+      <c r="G25" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="31"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1372,13 +1372,13 @@
       <c r="E26" s="17">
         <v>0.25</v>
       </c>
-      <c r="G26" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="J26" s="18"/>
+      <c r="G26" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" s="31"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
@@ -1391,16 +1391,16 @@
       <c r="E27" s="17">
         <v>0.25</v>
       </c>
-      <c r="G27" s="25" t="s">
+      <c r="G27" s="19" t="s">
         <v>61</v>
       </c>
       <c r="J27" s="15"/>
-      <c r="K27" s="18">
+      <c r="K27" s="31">
         <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="17" t="s">
         <v>22</v>
       </c>
@@ -1413,13 +1413,13 @@
       <c r="E28" s="17">
         <v>0.25</v>
       </c>
-      <c r="G28" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="K28" s="18"/>
+      <c r="G28" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K28" s="31"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="17" t="s">
         <v>25</v>
       </c>
@@ -1432,13 +1432,13 @@
       <c r="E29" s="17">
         <v>0.25</v>
       </c>
-      <c r="G29" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="K29" s="18"/>
+      <c r="G29" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29" s="31"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="17" t="s">
         <v>26</v>
       </c>
@@ -1451,10 +1451,10 @@
       <c r="E30" s="17">
         <v>0.25</v>
       </c>
-      <c r="G30" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="K30" s="18"/>
+      <c r="G30" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K30" s="31"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -1464,10 +1464,10 @@
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
-      <c r="G31" s="28"/>
+      <c r="G31" s="22"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -1482,10 +1482,10 @@
       <c r="E32" s="7">
         <v>0.25</v>
       </c>
-      <c r="G32" s="28"/>
+      <c r="G32" s="22"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="7" t="s">
         <v>22</v>
       </c>
@@ -1498,10 +1498,10 @@
       <c r="E33" s="7">
         <v>0.25</v>
       </c>
-      <c r="G33" s="28"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="7" t="s">
         <v>26</v>
       </c>
@@ -1514,10 +1514,10 @@
       <c r="E34" s="7">
         <v>0.25</v>
       </c>
-      <c r="G34" s="28"/>
+      <c r="G34" s="22"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="7" t="s">
         <v>46</v>
       </c>
@@ -1530,10 +1530,10 @@
       <c r="E35" s="7">
         <v>0.25</v>
       </c>
-      <c r="G35" s="28"/>
+      <c r="G35" s="22"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="7" t="s">
         <v>27</v>
       </c>
@@ -1546,10 +1546,10 @@
       <c r="E36" s="7">
         <v>0.25</v>
       </c>
-      <c r="G36" s="28"/>
+      <c r="G36" s="22"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="7" t="s">
         <v>44</v>
       </c>
@@ -1562,10 +1562,10 @@
       <c r="E37" s="7">
         <v>0.25</v>
       </c>
-      <c r="G37" s="28"/>
+      <c r="G37" s="22"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="7" t="s">
         <v>23</v>
       </c>
@@ -1578,10 +1578,10 @@
       <c r="E38" s="7">
         <v>0.25</v>
       </c>
-      <c r="G38" s="28"/>
+      <c r="G38" s="22"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="7" t="s">
         <v>28</v>
       </c>
@@ -1594,10 +1594,10 @@
       <c r="E39" s="7">
         <v>0.25</v>
       </c>
-      <c r="G39" s="28"/>
+      <c r="G39" s="22"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="7" t="s">
         <v>29</v>
       </c>
@@ -1610,10 +1610,10 @@
       <c r="E40" s="7">
         <v>0.25</v>
       </c>
-      <c r="G40" s="28"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="7" t="s">
         <v>30</v>
       </c>
@@ -1626,7 +1626,7 @@
       <c r="E41" s="7">
         <v>0.25</v>
       </c>
-      <c r="G41" s="28"/>
+      <c r="G41" s="22"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -1636,10 +1636,10 @@
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
-      <c r="G42" s="28"/>
+      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -1654,10 +1654,10 @@
       <c r="E43" s="7">
         <v>0.25</v>
       </c>
-      <c r="G43" s="28"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="7" t="s">
         <v>22</v>
       </c>
@@ -1670,10 +1670,10 @@
       <c r="E44" s="7">
         <v>0.25</v>
       </c>
-      <c r="G44" s="28"/>
+      <c r="G44" s="22"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="7" t="s">
         <v>26</v>
       </c>
@@ -1686,10 +1686,10 @@
       <c r="E45" s="7">
         <v>0.25</v>
       </c>
-      <c r="G45" s="28"/>
+      <c r="G45" s="22"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="7" t="s">
         <v>46</v>
       </c>
@@ -1702,10 +1702,10 @@
       <c r="E46" s="7">
         <v>0.25</v>
       </c>
-      <c r="G46" s="28"/>
+      <c r="G46" s="22"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="7" t="s">
         <v>27</v>
       </c>
@@ -1718,10 +1718,10 @@
       <c r="E47" s="7">
         <v>0.25</v>
       </c>
-      <c r="G47" s="28"/>
+      <c r="G47" s="22"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="7" t="s">
         <v>44</v>
       </c>
@@ -1734,10 +1734,10 @@
       <c r="E48" s="7">
         <v>0.25</v>
       </c>
-      <c r="G48" s="28"/>
+      <c r="G48" s="22"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="7" t="s">
         <v>23</v>
       </c>
@@ -1750,10 +1750,10 @@
       <c r="E49" s="7">
         <v>0.25</v>
       </c>
-      <c r="G49" s="28"/>
+      <c r="G49" s="22"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="7" t="s">
         <v>28</v>
       </c>
@@ -1766,10 +1766,10 @@
       <c r="E50" s="7">
         <v>0.25</v>
       </c>
-      <c r="G50" s="28"/>
+      <c r="G50" s="22"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
+      <c r="A51" s="29"/>
       <c r="B51" s="7" t="s">
         <v>29</v>
       </c>
@@ -1782,10 +1782,10 @@
       <c r="E51" s="7">
         <v>0.25</v>
       </c>
-      <c r="G51" s="28"/>
+      <c r="G51" s="22"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="7" t="s">
         <v>30</v>
       </c>
@@ -1798,10 +1798,10 @@
       <c r="E52" s="7">
         <v>0.25</v>
       </c>
-      <c r="G52" s="28"/>
+      <c r="G52" s="22"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="28" t="s">
         <v>11</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -1816,10 +1816,10 @@
       <c r="E53" s="8">
         <v>1</v>
       </c>
-      <c r="G53" s="28"/>
+      <c r="G53" s="22"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
+      <c r="A54" s="29"/>
       <c r="B54" s="8" t="s">
         <v>48</v>
       </c>
@@ -1832,10 +1832,10 @@
       <c r="E54" s="8">
         <v>1</v>
       </c>
-      <c r="G54" s="28"/>
+      <c r="G54" s="22"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
+      <c r="A55" s="29"/>
       <c r="B55" s="8" t="s">
         <v>42</v>
       </c>
@@ -1846,10 +1846,10 @@
       <c r="E55" s="8">
         <v>1</v>
       </c>
-      <c r="G55" s="28"/>
+      <c r="G55" s="22"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="21"/>
+      <c r="A56" s="30"/>
       <c r="B56" s="8" t="s">
         <v>38</v>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="E56" s="8">
         <v>1</v>
       </c>
-      <c r="G56" s="28"/>
+      <c r="G56" s="22"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -1880,7 +1880,7 @@
       <c r="E57" s="10">
         <v>2</v>
       </c>
-      <c r="G57" s="28"/>
+      <c r="G57" s="22"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
@@ -1890,10 +1890,10 @@
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
-      <c r="G58" s="28"/>
+      <c r="G58" s="22"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B59" s="11" t="s">
@@ -1908,10 +1908,10 @@
       <c r="E59" s="11">
         <v>2</v>
       </c>
-      <c r="G59" s="28"/>
+      <c r="G59" s="22"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="11" t="s">
         <v>52</v>
       </c>
@@ -1924,10 +1924,10 @@
       <c r="E60" s="11">
         <v>1</v>
       </c>
-      <c r="G60" s="28"/>
+      <c r="G60" s="22"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G61" s="28"/>
+      <c r="G61" s="22"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D62" s="6" t="s">
@@ -1940,51 +1940,51 @@
       <c r="F62" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G62" s="29"/>
+      <c r="G62" s="23"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G63" s="28"/>
+      <c r="G63" s="22"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G64" s="28"/>
+      <c r="G64" s="22"/>
     </row>
     <row r="65" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G65" s="28"/>
+      <c r="G65" s="22"/>
     </row>
     <row r="66" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G66" s="28"/>
+      <c r="G66" s="22"/>
     </row>
     <row r="67" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G67" s="28"/>
+      <c r="G67" s="22"/>
     </row>
     <row r="68" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G68" s="28"/>
+      <c r="G68" s="22"/>
     </row>
     <row r="69" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G69" s="28"/>
+      <c r="G69" s="22"/>
     </row>
     <row r="70" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G70" s="28"/>
+      <c r="G70" s="22"/>
     </row>
     <row r="71" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G71" s="28"/>
+      <c r="G71" s="22"/>
     </row>
     <row r="72" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G72" s="28"/>
+      <c r="G72" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="K27:K30"/>
+    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="A53:A56"/>
     <mergeCell ref="L6:L13"/>
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A30"/>
-    <mergeCell ref="A32:A41"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="K27:K30"/>
-    <mergeCell ref="A43:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A59:A60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update dues-in and ro
</commit_message>
<xml_diff>
--- a/kms/HIS-2396/HIS-2396 - Update Transaction Status List v0.2.xlsx
+++ b/kms/HIS-2396/HIS-2396 - Update Transaction Status List v0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MySpace\PMS\kms\HIS-2396\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCB3E97-551D-494D-B227-22275F108539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB10D592-0AE7-45BB-8897-D3DD20F57007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{F92CBCCC-CE4E-451F-B585-C555BA546955}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="66">
   <si>
     <t>A. In transit</t>
   </si>
@@ -227,14 +227,17 @@
     <t>status (create query)</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>I will do this case after update data for dues-in PO</t>
+  </si>
+  <si>
+    <t>wait for update dues-in PO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,13 +269,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -413,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -443,7 +439,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -453,15 +451,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,9 +776,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F4FEA4-F864-45AA-AF75-3534CC6ADEA0}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AF72"/>
+  <dimension ref="A1:AD72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -794,14 +789,15 @@
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="32" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -839,67 +835,61 @@
         <v>43735</v>
       </c>
       <c r="M1" s="14">
-        <v>43736</v>
+        <v>43738</v>
       </c>
       <c r="N1" s="14">
-        <v>43737</v>
+        <v>43739</v>
       </c>
       <c r="O1" s="14">
-        <v>43738</v>
+        <v>43740</v>
       </c>
       <c r="P1" s="14">
-        <v>43739</v>
+        <v>43741</v>
       </c>
       <c r="Q1" s="14">
-        <v>43740</v>
+        <v>43742</v>
       </c>
       <c r="R1" s="14">
-        <v>43741</v>
+        <v>43743</v>
       </c>
       <c r="S1" s="14">
-        <v>43742</v>
+        <v>43744</v>
       </c>
       <c r="T1" s="14">
-        <v>43743</v>
+        <v>43745</v>
       </c>
       <c r="U1" s="14">
-        <v>43744</v>
+        <v>43746</v>
       </c>
       <c r="V1" s="14">
-        <v>43745</v>
+        <v>43747</v>
       </c>
       <c r="W1" s="14">
-        <v>43746</v>
+        <v>43748</v>
       </c>
       <c r="X1" s="14">
-        <v>43747</v>
+        <v>43749</v>
       </c>
       <c r="Y1" s="14">
-        <v>43748</v>
+        <v>43750</v>
       </c>
       <c r="Z1" s="14">
-        <v>43749</v>
+        <v>43751</v>
       </c>
       <c r="AA1" s="14">
-        <v>43750</v>
+        <v>43752</v>
       </c>
       <c r="AB1" s="14">
-        <v>43751</v>
+        <v>43753</v>
       </c>
       <c r="AC1" s="14">
-        <v>43752</v>
+        <v>43754</v>
       </c>
       <c r="AD1" s="14">
-        <v>43753</v>
-      </c>
-      <c r="AE1" s="14">
-        <v>43754</v>
-      </c>
-      <c r="AF1" s="14">
         <v>43755</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -909,7 +899,7 @@
       <c r="E2" s="4"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -927,7 +917,7 @@
       </c>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -937,7 +927,7 @@
       <c r="E4" s="4"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -953,16 +943,18 @@
       <c r="E5" s="12">
         <v>2</v>
       </c>
-      <c r="G5" s="22"/>
+      <c r="G5" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="K5">
         <v>0.25</v>
       </c>
       <c r="L5">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -983,12 +975,12 @@
       <c r="G6" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="30">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="M6" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
       <c r="B7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1004,10 +996,10 @@
       <c r="G7" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="30"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="M7" s="25"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1023,10 +1015,10 @@
       <c r="G8" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L8" s="30"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="M8" s="25"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
       <c r="B9" s="7" t="s">
         <v>28</v>
       </c>
@@ -1042,10 +1034,10 @@
       <c r="G9" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L9" s="30"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="M9" s="25"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
       <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
@@ -1061,10 +1053,10 @@
       <c r="G10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="30"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="M10" s="25"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
       <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
@@ -1080,10 +1072,10 @@
       <c r="G11" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L11" s="30"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="M11" s="25"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
       <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1099,10 +1091,10 @@
       <c r="G12" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="30"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="M12" s="25"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
       <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1118,9 +1110,9 @@
       <c r="G13" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="30"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="M13" s="25"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1136,11 +1128,17 @@
       <c r="E14" s="11">
         <v>2</v>
       </c>
-      <c r="G14" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="G14" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14">
+        <v>0.5</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -1150,8 +1148,8 @@
       <c r="E15" s="4"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -1174,7 +1172,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="16" t="s">
         <v>37</v>
       </c>
@@ -1192,7 +1190,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="16" t="s">
         <v>38</v>
       </c>
@@ -1210,7 +1208,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="16" t="s">
         <v>17</v>
       </c>
@@ -1228,7 +1226,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1249,7 +1247,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="16" t="s">
         <v>32</v>
       </c>
@@ -1267,7 +1265,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="16" t="s">
         <v>23</v>
       </c>
@@ -1285,7 +1283,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -1317,7 +1315,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="17" t="s">
         <v>30</v>
       </c>
@@ -1333,12 +1331,12 @@
       <c r="G24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J24" s="29">
+      <c r="J24" s="25">
         <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="17" t="s">
         <v>23</v>
       </c>
@@ -1354,10 +1352,10 @@
       <c r="G25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J25" s="29"/>
+      <c r="J25" s="25"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1373,10 +1371,10 @@
       <c r="G26" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="29"/>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
@@ -1393,12 +1391,12 @@
         <v>61</v>
       </c>
       <c r="J27" s="15"/>
-      <c r="K27" s="29">
+      <c r="K27" s="25">
         <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="17" t="s">
         <v>22</v>
       </c>
@@ -1414,10 +1412,10 @@
       <c r="G28" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K28" s="29"/>
+      <c r="K28" s="25"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="17" t="s">
         <v>25</v>
       </c>
@@ -1433,10 +1431,10 @@
       <c r="G29" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K29" s="29"/>
+      <c r="K29" s="25"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="17" t="s">
         <v>26</v>
       </c>
@@ -1452,7 +1450,7 @@
       <c r="G30" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K30" s="29"/>
+      <c r="K30" s="25"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -1734,7 +1732,7 @@
       </c>
       <c r="G48" s="22"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
       <c r="B49" s="7" t="s">
         <v>23</v>
@@ -1750,7 +1748,7 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="28"/>
       <c r="B50" s="7" t="s">
         <v>28</v>
@@ -1766,7 +1764,7 @@
       </c>
       <c r="G50" s="22"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="28"/>
       <c r="B51" s="7" t="s">
         <v>29</v>
@@ -1782,7 +1780,7 @@
       </c>
       <c r="G51" s="22"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="27"/>
       <c r="B52" s="7" t="s">
         <v>30</v>
@@ -1798,7 +1796,7 @@
       </c>
       <c r="G52" s="22"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
         <v>11</v>
       </c>
@@ -1816,7 +1814,7 @@
       </c>
       <c r="G53" s="22"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="28"/>
       <c r="B54" s="8" t="s">
         <v>48</v>
@@ -1832,7 +1830,7 @@
       </c>
       <c r="G54" s="22"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="28"/>
       <c r="B55" s="8" t="s">
         <v>42</v>
@@ -1846,7 +1844,7 @@
       </c>
       <c r="G55" s="22"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="27"/>
       <c r="B56" s="8" t="s">
         <v>38</v>
@@ -1862,7 +1860,7 @@
       </c>
       <c r="G56" s="22"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>12</v>
       </c>
@@ -1880,7 +1878,7 @@
       </c>
       <c r="G57" s="22"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>13</v>
       </c>
@@ -1890,7 +1888,7 @@
       <c r="E58" s="4"/>
       <c r="G58" s="22"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="26" t="s">
         <v>14</v>
       </c>
@@ -1906,9 +1904,14 @@
       <c r="E59" s="11">
         <v>2</v>
       </c>
-      <c r="G59" s="22"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="27"/>
       <c r="B60" s="11" t="s">
         <v>52</v>
@@ -1922,12 +1925,17 @@
       <c r="E60" s="11">
         <v>1</v>
       </c>
-      <c r="G60" s="22"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F60" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G60" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G61" s="22"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D62" s="6" t="s">
         <v>55</v>
       </c>
@@ -1940,10 +1948,10 @@
       </c>
       <c r="G62" s="23"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G63" s="22"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G64" s="22"/>
     </row>
     <row r="65" spans="7:7" x14ac:dyDescent="0.25">
@@ -1972,17 +1980,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="L6:L13"/>
-    <mergeCell ref="A6:A13"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="M6:M13"/>
     <mergeCell ref="A59:A60"/>
     <mergeCell ref="A32:A41"/>
     <mergeCell ref="J24:J26"/>
     <mergeCell ref="K27:K30"/>
     <mergeCell ref="A43:A52"/>
     <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
create query outstanding-out medication chart and update query to get list data.
</commit_message>
<xml_diff>
--- a/kms/HIS-2396/HIS-2396 - Update Transaction Status List v0.2.xlsx
+++ b/kms/HIS-2396/HIS-2396 - Update Transaction Status List v0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MySpace\PMS\kms\HIS-2396\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E518A7-06AC-47B3-B1D9-2FD33AFF0487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EE293F-55E9-4FA9-9DB2-AD547A67DB97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{F92CBCCC-CE4E-451F-B585-C555BA546955}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="73">
   <si>
     <t>A. In transit</t>
   </si>
@@ -245,7 +245,13 @@
     <t>less than 10 records, should do it manually</t>
   </si>
   <si>
-    <t>there is no record, maybe they are updated in dues-out</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>in-progress, wait for replication</t>
+  </si>
+  <si>
+    <t>Cannot unclaimed prescription since the status is not ALLOCATED. There is no records, maybe they were updated in dues-out.</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -458,8 +464,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -473,12 +480,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,9 +804,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F4FEA4-F864-45AA-AF75-3534CC6ADEA0}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AB72"/>
+  <dimension ref="A1:Z72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -822,10 +826,12 @@
     <col min="18" max="18" width="5.5703125" customWidth="1"/>
     <col min="19" max="19" width="4.85546875" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.85546875" customWidth="1"/>
+    <col min="23" max="23" width="6.28515625" customWidth="1"/>
+    <col min="24" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -893,25 +899,19 @@
         <v>43749</v>
       </c>
       <c r="W1" s="14">
-        <v>43750</v>
+        <v>43752</v>
       </c>
       <c r="X1" s="14">
-        <v>43751</v>
+        <v>43753</v>
       </c>
       <c r="Y1" s="14">
-        <v>43752</v>
+        <v>43754</v>
       </c>
       <c r="Z1" s="14">
-        <v>43753</v>
-      </c>
-      <c r="AA1" s="14">
-        <v>43754</v>
-      </c>
-      <c r="AB1" s="14">
         <v>43755</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -921,7 +921,7 @@
       <c r="E2" s="4"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -937,14 +937,12 @@
       <c r="E3" s="13">
         <v>2</v>
       </c>
-      <c r="F3" s="37" t="s">
-        <v>69</v>
-      </c>
+      <c r="F3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -954,7 +952,7 @@
       <c r="E4" s="4"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -980,8 +978,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1002,12 +1000,12 @@
       <c r="G6" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M6" s="30">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
       <c r="B7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1023,10 +1021,10 @@
       <c r="G7" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M7" s="34"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="M7" s="30"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1042,10 +1040,10 @@
       <c r="G8" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M8" s="34"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="M8" s="30"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
       <c r="B9" s="7" t="s">
         <v>28</v>
       </c>
@@ -1061,10 +1059,10 @@
       <c r="G9" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M9" s="34"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="M9" s="30"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
       <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
@@ -1080,10 +1078,10 @@
       <c r="G10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M10" s="34"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="M10" s="30"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
       <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
@@ -1099,10 +1097,10 @@
       <c r="G11" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="34"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="M11" s="30"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
       <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1118,10 +1116,10 @@
       <c r="G12" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M12" s="34"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="M12" s="30"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
       <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1137,9 +1135,9 @@
       <c r="G13" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="34"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="M13" s="30"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1165,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -1175,8 +1173,8 @@
       <c r="E15" s="4"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -1199,7 +1197,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="16" t="s">
         <v>37</v>
       </c>
@@ -1217,7 +1215,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="16" t="s">
         <v>38</v>
       </c>
@@ -1235,7 +1233,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="16" t="s">
         <v>17</v>
       </c>
@@ -1253,7 +1251,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1274,7 +1272,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="16" t="s">
         <v>32</v>
       </c>
@@ -1292,7 +1290,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="16" t="s">
         <v>23</v>
       </c>
@@ -1310,7 +1308,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="35" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -1342,7 +1340,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="17" t="s">
         <v>30</v>
       </c>
@@ -1358,12 +1356,12 @@
       <c r="G24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J24" s="34">
+      <c r="J24" s="30">
         <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="17" t="s">
         <v>23</v>
       </c>
@@ -1379,10 +1377,10 @@
       <c r="G25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J25" s="34"/>
+      <c r="J25" s="30"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1398,10 +1396,10 @@
       <c r="G26" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="34"/>
+      <c r="J26" s="30"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
@@ -1418,12 +1416,12 @@
         <v>61</v>
       </c>
       <c r="J27" s="15"/>
-      <c r="K27" s="34">
+      <c r="K27" s="30">
         <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="17" t="s">
         <v>22</v>
       </c>
@@ -1439,10 +1437,10 @@
       <c r="G28" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K28" s="34"/>
+      <c r="K28" s="30"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="17" t="s">
         <v>25</v>
       </c>
@@ -1458,10 +1456,10 @@
       <c r="G29" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K29" s="34"/>
+      <c r="K29" s="30"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="17" t="s">
         <v>26</v>
       </c>
@@ -1477,7 +1475,7 @@
       <c r="G30" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K30" s="34"/>
+      <c r="K30" s="30"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -1490,7 +1488,7 @@
       <c r="G31" s="22"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -1505,18 +1503,18 @@
       <c r="E32" s="7">
         <v>0.25</v>
       </c>
-      <c r="G32" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="P32" s="34">
+      <c r="G32" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="P32" s="30">
         <v>1</v>
       </c>
-      <c r="Q32" s="34">
+      <c r="Q32" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="7" t="s">
         <v>22</v>
       </c>
@@ -1529,12 +1527,12 @@
       <c r="E33" s="7">
         <v>0.25</v>
       </c>
-      <c r="G33" s="30"/>
-      <c r="P33" s="34"/>
-      <c r="Q33" s="34"/>
+      <c r="G33" s="31"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="7" t="s">
         <v>26</v>
       </c>
@@ -1547,12 +1545,12 @@
       <c r="E34" s="7">
         <v>0.25</v>
       </c>
-      <c r="G34" s="30"/>
-      <c r="P34" s="34"/>
-      <c r="Q34" s="34"/>
+      <c r="G34" s="31"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="30"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="7" t="s">
         <v>46</v>
       </c>
@@ -1568,12 +1566,12 @@
       <c r="F35" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="30"/>
-      <c r="P35" s="34"/>
-      <c r="Q35" s="34"/>
+      <c r="G35" s="31"/>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="30"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="7" t="s">
         <v>27</v>
       </c>
@@ -1586,12 +1584,12 @@
       <c r="E36" s="7">
         <v>0.25</v>
       </c>
-      <c r="G36" s="30"/>
-      <c r="P36" s="34"/>
-      <c r="Q36" s="34"/>
+      <c r="G36" s="31"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="7" t="s">
         <v>44</v>
       </c>
@@ -1604,12 +1602,12 @@
       <c r="E37" s="7">
         <v>0.25</v>
       </c>
-      <c r="G37" s="30"/>
-      <c r="P37" s="34"/>
-      <c r="Q37" s="34"/>
+      <c r="G37" s="31"/>
+      <c r="P37" s="30"/>
+      <c r="Q37" s="30"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="7" t="s">
         <v>23</v>
       </c>
@@ -1622,12 +1620,12 @@
       <c r="E38" s="7">
         <v>0.25</v>
       </c>
-      <c r="G38" s="30"/>
-      <c r="P38" s="34"/>
-      <c r="Q38" s="34"/>
+      <c r="G38" s="31"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="7" t="s">
         <v>28</v>
       </c>
@@ -1640,12 +1638,12 @@
       <c r="E39" s="7">
         <v>0.25</v>
       </c>
-      <c r="G39" s="30"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
+      <c r="G39" s="31"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="7" t="s">
         <v>29</v>
       </c>
@@ -1658,12 +1656,12 @@
       <c r="E40" s="7">
         <v>0.25</v>
       </c>
-      <c r="G40" s="30"/>
-      <c r="P40" s="34"/>
-      <c r="Q40" s="34"/>
+      <c r="G40" s="31"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="33"/>
       <c r="B41" s="7" t="s">
         <v>30</v>
       </c>
@@ -1676,9 +1674,9 @@
       <c r="E41" s="7">
         <v>0.25</v>
       </c>
-      <c r="G41" s="30"/>
-      <c r="P41" s="34"/>
-      <c r="Q41" s="34"/>
+      <c r="G41" s="31"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -1691,7 +1689,7 @@
       <c r="G42" s="22"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -1706,15 +1704,15 @@
       <c r="E43" s="7">
         <v>0.25</v>
       </c>
-      <c r="G43" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="R43" s="34">
+      <c r="G43" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="R43" s="30">
         <v>0.75</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
+      <c r="A44" s="34"/>
       <c r="B44" s="7" t="s">
         <v>22</v>
       </c>
@@ -1727,11 +1725,11 @@
       <c r="E44" s="7">
         <v>0.25</v>
       </c>
-      <c r="G44" s="30"/>
-      <c r="R44" s="34"/>
+      <c r="G44" s="31"/>
+      <c r="R44" s="30"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
+      <c r="A45" s="34"/>
       <c r="B45" s="7" t="s">
         <v>26</v>
       </c>
@@ -1744,11 +1742,11 @@
       <c r="E45" s="7">
         <v>0.25</v>
       </c>
-      <c r="G45" s="30"/>
-      <c r="R45" s="34"/>
+      <c r="G45" s="31"/>
+      <c r="R45" s="30"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
+      <c r="A46" s="34"/>
       <c r="B46" s="26" t="s">
         <v>46</v>
       </c>
@@ -1764,11 +1762,11 @@
       <c r="F46" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="G46" s="30"/>
-      <c r="R46" s="34"/>
+      <c r="G46" s="31"/>
+      <c r="R46" s="30"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="33"/>
+      <c r="A47" s="34"/>
       <c r="B47" s="7" t="s">
         <v>27</v>
       </c>
@@ -1781,11 +1779,11 @@
       <c r="E47" s="7">
         <v>0.25</v>
       </c>
-      <c r="G47" s="30"/>
-      <c r="R47" s="34"/>
+      <c r="G47" s="31"/>
+      <c r="R47" s="30"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
+      <c r="A48" s="34"/>
       <c r="B48" s="26" t="s">
         <v>44</v>
       </c>
@@ -1798,11 +1796,11 @@
       <c r="E48" s="26">
         <v>0.25</v>
       </c>
-      <c r="G48" s="30"/>
-      <c r="R48" s="34"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="G48" s="31"/>
+      <c r="R48" s="30"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A49" s="34"/>
       <c r="B49" s="7" t="s">
         <v>23</v>
       </c>
@@ -1815,11 +1813,11 @@
       <c r="E49" s="7">
         <v>0.25</v>
       </c>
-      <c r="G49" s="30"/>
-      <c r="R49" s="34"/>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
+      <c r="G49" s="31"/>
+      <c r="R49" s="30"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A50" s="34"/>
       <c r="B50" s="7" t="s">
         <v>28</v>
       </c>
@@ -1832,11 +1830,11 @@
       <c r="E50" s="7">
         <v>0.25</v>
       </c>
-      <c r="G50" s="30"/>
-      <c r="R50" s="34"/>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="33"/>
+      <c r="G50" s="31"/>
+      <c r="R50" s="30"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A51" s="34"/>
       <c r="B51" s="7" t="s">
         <v>29</v>
       </c>
@@ -1849,11 +1847,11 @@
       <c r="E51" s="7">
         <v>0.25</v>
       </c>
-      <c r="G51" s="30"/>
-      <c r="R51" s="34"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
+      <c r="G51" s="31"/>
+      <c r="R51" s="30"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A52" s="33"/>
       <c r="B52" s="7" t="s">
         <v>30</v>
       </c>
@@ -1866,11 +1864,11 @@
       <c r="E52" s="7">
         <v>0.25</v>
       </c>
-      <c r="G52" s="30"/>
-      <c r="R52" s="34"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="31" t="s">
+      <c r="G52" s="31"/>
+      <c r="R52" s="30"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -1885,7 +1883,7 @@
       <c r="E53" s="8">
         <v>1</v>
       </c>
-      <c r="F53" s="35" t="s">
+      <c r="F53" s="29" t="s">
         <v>69</v>
       </c>
       <c r="G53" s="19" t="s">
@@ -1898,8 +1896,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A54" s="34"/>
       <c r="B54" s="8" t="s">
         <v>48</v>
       </c>
@@ -1913,11 +1911,14 @@
         <v>1</v>
       </c>
       <c r="G54" s="28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
+        <v>71</v>
+      </c>
+      <c r="T54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A55" s="34"/>
       <c r="B55" s="8" t="s">
         <v>42</v>
       </c>
@@ -1938,8 +1939,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A56" s="32"/>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A56" s="33"/>
       <c r="B56" s="8" t="s">
         <v>38</v>
       </c>
@@ -1952,14 +1953,23 @@
       <c r="E56" s="8">
         <v>1</v>
       </c>
-      <c r="F56" s="35" t="s">
+      <c r="F56" t="s">
+        <v>72</v>
+      </c>
+      <c r="G56" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N56" t="s">
         <v>70</v>
       </c>
-      <c r="G56" s="35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T56">
+        <v>0.5</v>
+      </c>
+      <c r="U56">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>12</v>
       </c>
@@ -1975,14 +1985,20 @@
       <c r="E57" s="10">
         <v>2</v>
       </c>
-      <c r="F57" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="G57" s="36" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G57" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="U57">
+        <v>0.5</v>
+      </c>
+      <c r="V57">
+        <v>1</v>
+      </c>
+      <c r="W57">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>13</v>
       </c>
@@ -1992,8 +2008,8 @@
       <c r="E58" s="4"/>
       <c r="G58" s="22"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
         <v>14</v>
       </c>
       <c r="B59" s="11" t="s">
@@ -2015,8 +2031,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A60" s="33"/>
       <c r="B60" s="11" t="s">
         <v>52</v>
       </c>
@@ -2036,10 +2052,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G61" s="22"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D62" s="6" t="s">
         <v>55</v>
       </c>
@@ -2052,10 +2068,10 @@
       </c>
       <c r="G62" s="23"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G63" s="22"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G64" s="22"/>
     </row>
     <row r="65" spans="7:7" x14ac:dyDescent="0.25">
@@ -2084,22 +2100,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="R43:R52"/>
-    <mergeCell ref="P32:P41"/>
-    <mergeCell ref="G32:G41"/>
-    <mergeCell ref="Q32:Q41"/>
-    <mergeCell ref="M6:M13"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="G43:G52"/>
     <mergeCell ref="A59:A60"/>
     <mergeCell ref="A32:A41"/>
     <mergeCell ref="J24:J26"/>
     <mergeCell ref="K27:K30"/>
     <mergeCell ref="A43:A52"/>
     <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A6:A13"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="G43:G52"/>
+    <mergeCell ref="R43:R52"/>
+    <mergeCell ref="P32:P41"/>
+    <mergeCell ref="G32:G41"/>
+    <mergeCell ref="Q32:Q41"/>
+    <mergeCell ref="M6:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
create query for in-transit
</commit_message>
<xml_diff>
--- a/kms/HIS-2396/HIS-2396 - Update Transaction Status List v0.2.xlsx
+++ b/kms/HIS-2396/HIS-2396 - Update Transaction Status List v0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MySpace\PMS\kms\HIS-2396\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EE293F-55E9-4FA9-9DB2-AD547A67DB97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3819C15A-288E-454A-AE93-CC7E6534FD9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{F92CBCCC-CE4E-451F-B585-C555BA546955}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="72">
   <si>
     <t>A. In transit</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>wait for update dues-in PO</t>
-  </si>
-  <si>
-    <t>in-progress</t>
   </si>
   <si>
     <t>should do it manually</t>
@@ -465,8 +462,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -480,8 +477,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -939,7 +936,10 @@
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="W3">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="30" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1000,12 +1000,12 @@
       <c r="G6" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1021,10 +1021,10 @@
       <c r="G7" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M7" s="30"/>
+      <c r="M7" s="35"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1040,10 +1040,10 @@
       <c r="G8" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M8" s="30"/>
+      <c r="M8" s="35"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="7" t="s">
         <v>28</v>
       </c>
@@ -1059,10 +1059,10 @@
       <c r="G9" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M9" s="30"/>
+      <c r="M9" s="35"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
@@ -1078,10 +1078,10 @@
       <c r="G10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M10" s="30"/>
+      <c r="M10" s="35"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
@@ -1097,10 +1097,10 @@
       <c r="G11" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="30"/>
+      <c r="M11" s="35"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1116,10 +1116,10 @@
       <c r="G12" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M12" s="30"/>
+      <c r="M12" s="35"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="G13" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="30"/>
+      <c r="M13" s="35"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1174,7 +1174,7 @@
       <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -1197,7 +1197,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="16" t="s">
         <v>37</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="16" t="s">
         <v>38</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="16" t="s">
         <v>17</v>
       </c>
@@ -1251,7 +1251,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="30" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1272,7 +1272,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="16" t="s">
         <v>32</v>
       </c>
@@ -1290,7 +1290,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="16" t="s">
         <v>23</v>
       </c>
@@ -1308,7 +1308,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -1340,7 +1340,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="17" t="s">
         <v>30</v>
       </c>
@@ -1356,12 +1356,12 @@
       <c r="G24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J24" s="30">
+      <c r="J24" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="17" t="s">
         <v>23</v>
       </c>
@@ -1377,10 +1377,10 @@
       <c r="G25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J25" s="30"/>
+      <c r="J25" s="35"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1396,10 +1396,10 @@
       <c r="G26" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="30"/>
+      <c r="J26" s="35"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
@@ -1416,12 +1416,12 @@
         <v>61</v>
       </c>
       <c r="J27" s="15"/>
-      <c r="K27" s="30">
+      <c r="K27" s="35">
         <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="17" t="s">
         <v>22</v>
       </c>
@@ -1437,10 +1437,10 @@
       <c r="G28" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K28" s="30"/>
+      <c r="K28" s="35"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="17" t="s">
         <v>25</v>
       </c>
@@ -1456,10 +1456,10 @@
       <c r="G29" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K29" s="30"/>
+      <c r="K29" s="35"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="17" t="s">
         <v>26</v>
       </c>
@@ -1475,7 +1475,7 @@
       <c r="G30" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K30" s="30"/>
+      <c r="K30" s="35"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -1506,10 +1506,10 @@
       <c r="G32" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="P32" s="30">
+      <c r="P32" s="35">
         <v>1</v>
       </c>
-      <c r="Q32" s="30">
+      <c r="Q32" s="35">
         <v>1</v>
       </c>
     </row>
@@ -1528,8 +1528,8 @@
         <v>0.25</v>
       </c>
       <c r="G33" s="31"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
@@ -1546,8 +1546,8 @@
         <v>0.25</v>
       </c>
       <c r="G34" s="31"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
@@ -1564,11 +1564,11 @@
         <v>0.25</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35" s="31"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="30"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="34"/>
@@ -1585,8 +1585,8 @@
         <v>0.25</v>
       </c>
       <c r="G36" s="31"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="34"/>
@@ -1603,8 +1603,8 @@
         <v>0.25</v>
       </c>
       <c r="G37" s="31"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="34"/>
@@ -1621,8 +1621,8 @@
         <v>0.25</v>
       </c>
       <c r="G38" s="31"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
@@ -1639,8 +1639,8 @@
         <v>0.25</v>
       </c>
       <c r="G39" s="31"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
@@ -1657,8 +1657,8 @@
         <v>0.25</v>
       </c>
       <c r="G40" s="31"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="33"/>
@@ -1675,8 +1675,8 @@
         <v>0.25</v>
       </c>
       <c r="G41" s="31"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -1707,7 +1707,7 @@
       <c r="G43" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="R43" s="30">
+      <c r="R43" s="35">
         <v>0.75</v>
       </c>
     </row>
@@ -1726,7 +1726,7 @@
         <v>0.25</v>
       </c>
       <c r="G44" s="31"/>
-      <c r="R44" s="30"/>
+      <c r="R44" s="35"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="34"/>
@@ -1743,7 +1743,7 @@
         <v>0.25</v>
       </c>
       <c r="G45" s="31"/>
-      <c r="R45" s="30"/>
+      <c r="R45" s="35"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="34"/>
@@ -1760,10 +1760,10 @@
         <v>0.25</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G46" s="31"/>
-      <c r="R46" s="30"/>
+      <c r="R46" s="35"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="34"/>
@@ -1780,7 +1780,7 @@
         <v>0.25</v>
       </c>
       <c r="G47" s="31"/>
-      <c r="R47" s="30"/>
+      <c r="R47" s="35"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="34"/>
@@ -1797,7 +1797,7 @@
         <v>0.25</v>
       </c>
       <c r="G48" s="31"/>
-      <c r="R48" s="30"/>
+      <c r="R48" s="35"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="34"/>
@@ -1814,7 +1814,7 @@
         <v>0.25</v>
       </c>
       <c r="G49" s="31"/>
-      <c r="R49" s="30"/>
+      <c r="R49" s="35"/>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="34"/>
@@ -1831,7 +1831,7 @@
         <v>0.25</v>
       </c>
       <c r="G50" s="31"/>
-      <c r="R50" s="30"/>
+      <c r="R50" s="35"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="34"/>
@@ -1848,7 +1848,7 @@
         <v>0.25</v>
       </c>
       <c r="G51" s="31"/>
-      <c r="R51" s="30"/>
+      <c r="R51" s="35"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="33"/>
@@ -1865,7 +1865,7 @@
         <v>0.25</v>
       </c>
       <c r="G52" s="31"/>
-      <c r="R52" s="30"/>
+      <c r="R52" s="35"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G53" s="19" t="s">
         <v>61</v>
@@ -1911,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T54">
         <v>0.5</v>
@@ -1930,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G55" s="19" t="s">
         <v>61</v>
@@ -1954,13 +1954,13 @@
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G56" s="19" t="s">
         <v>61</v>
       </c>
       <c r="N56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T56">
         <v>0.5</v>
@@ -2100,22 +2100,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A6:A13"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="G43:G52"/>
+    <mergeCell ref="R43:R52"/>
+    <mergeCell ref="P32:P41"/>
+    <mergeCell ref="G32:G41"/>
+    <mergeCell ref="Q32:Q41"/>
+    <mergeCell ref="M6:M13"/>
     <mergeCell ref="A59:A60"/>
     <mergeCell ref="A32:A41"/>
     <mergeCell ref="J24:J26"/>
     <mergeCell ref="K27:K30"/>
     <mergeCell ref="A43:A52"/>
     <mergeCell ref="A53:A56"/>
-    <mergeCell ref="R43:R52"/>
-    <mergeCell ref="P32:P41"/>
-    <mergeCell ref="G32:G41"/>
-    <mergeCell ref="Q32:Q41"/>
-    <mergeCell ref="M6:M13"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="G43:G52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>